<commit_message>
Created build structure for the project
</commit_message>
<xml_diff>
--- a/prj/status.xlsx
+++ b/prj/status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\abhijit\intellij\lss\prj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91747C57-B6A8-48B7-8EDE-C37F915D42CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC85D6F2-D52E-4CE3-8F0F-C7E0BAC83FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -446,7 +446,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,13 +511,15 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
@@ -529,15 +531,13 @@
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">

</xml_diff>

<commit_message>
Dummy server service implementation.
</commit_message>
<xml_diff>
--- a/prj/status.xlsx
+++ b/prj/status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\abhijit\intellij\lss\prj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC85D6F2-D52E-4CE3-8F0F-C7E0BAC83FD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBA21FA-C1EE-4BF8-B7B5-583948ABE521}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>S.No.</t>
   </si>
@@ -57,17 +57,20 @@
     <t>Call server service from angular</t>
   </si>
   <si>
-    <t>Create build strategy</t>
-  </si>
-  <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Create project sturcture and build strategy</t>
+  </si>
+  <si>
+    <t>Integrate server service with database</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -98,6 +101,13 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -157,12 +167,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,16 +454,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -474,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -485,7 +496,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -496,7 +507,7 @@
         <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -507,7 +518,7 @@
         <v>6</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -518,17 +529,19 @@
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
@@ -544,11 +557,20 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>